<commit_message>
compare between excel and database
</commit_message>
<xml_diff>
--- a/projects/p1/data/nav-s2.xlsx
+++ b/projects/p1/data/nav-s2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/PycharmProjects/py_monorep/projects/p1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00537A67-5BBB-F14A-9F05-672E7ED98BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673048B7-EC98-7E48-883F-3362A185B1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15620" xr2:uid="{F2572F92-B09A-AA41-B13B-6C17FFA4F077}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15560" xr2:uid="{F2572F92-B09A-AA41-B13B-6C17FFA4F077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>navdate</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>070</t>
+  </si>
+  <si>
+    <t>fnd_ver</t>
+  </si>
+  <si>
+    <t>01</t>
   </si>
 </sst>
 </file>
@@ -420,15 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF625F6-820F-034D-AF48-9C199FD0D0FF}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,61 +442,79 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
         <v>12.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
         <v>13</v>
       </c>
     </row>

</xml_diff>